<commit_message>
Adding Select Destination Box
</commit_message>
<xml_diff>
--- a/public/Assets/files/ourDeals.xlsx
+++ b/public/Assets/files/ourDeals.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Programming for Job Hunt\08 - Top Tiulim\public\Assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3B8830E-4542-4D79-9535-BECB809514E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87ED2BCC-D94A-479D-8F55-764A34BB0C2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5760" yWindow="0" windowWidth="17280" windowHeight="8880" xr2:uid="{676D24D3-B49B-41D9-8CC8-E40E6709C598}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{676D24D3-B49B-41D9-8CC8-E40E6709C598}"/>
   </bookViews>
   <sheets>
     <sheet name="Deals" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="77">
   <si>
     <t>destination</t>
   </si>
@@ -70,9 +70,6 @@
   </si>
   <si>
     <t>טיול בג'ונגלים</t>
-  </si>
-  <si>
-    <t>דובאי, איחוד האמיריות</t>
   </si>
   <si>
     <t>ג'יפים וגמלים</t>
@@ -285,6 +282,24 @@
     { "type": "image", "url": "https://toptiulim.co.il/assets/galleryImgs/%D7%A2%D7%95%D7%AA%D7%A7%20%D7%A9%D7%9C%20IMG_1851.jpg" },
     { "type": "image", "url": "https://toptiulim.co.il/assets/galleryImgs/%D7%A2%D7%95%D7%AA%D7%A7%20%D7%A9%D7%9C%20IMG_1791.jpg" }
 ]</t>
+  </si>
+  <si>
+    <t>country</t>
+  </si>
+  <si>
+    <t>גאורגיה</t>
+  </si>
+  <si>
+    <t>תאילנד</t>
+  </si>
+  <si>
+    <t>דובאי, איחוד האמירויות</t>
+  </si>
+  <si>
+    <t>איחוד האמירויות</t>
+  </si>
+  <si>
+    <t>ישראל</t>
   </si>
 </sst>
 </file>
@@ -769,212 +784,233 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C1A6A43-A05D-49B0-8F71-05A6579839E1}">
-  <dimension ref="A1:I7"/>
+  <dimension ref="A1:J7"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="E1" zoomScale="88" zoomScaleNormal="63" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G7" sqref="G7"/>
+    <sheetView rightToLeft="1" tabSelected="1" zoomScale="88" zoomScaleNormal="63" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="9" width="25.69921875" style="1" customWidth="1"/>
-    <col min="10" max="23" width="5.69921875" style="1" customWidth="1"/>
-    <col min="24" max="16384" width="8.796875" style="1"/>
+    <col min="1" max="10" width="25.69921875" style="1" customWidth="1"/>
+    <col min="11" max="24" width="5.69921875" style="1" customWidth="1"/>
+    <col min="25" max="16384" width="8.796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>44</v>
+        <v>64</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" ht="331.8" thickTop="1" x14ac:dyDescent="0.25">
+        <v>43</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="331.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>12563</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F2" s="1">
+      <c r="G2" s="1">
         <v>3250</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>66</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="I2" s="2" t="b">
+        <v>65</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="J2" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="331.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:10" ht="331.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>12564</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F3" s="1">
+      <c r="G3" s="1">
         <v>4450</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>67</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="I3" s="2" t="b">
+        <v>66</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="J3" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="331.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" ht="331.2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>12565</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" s="2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F4" s="1">
+      <c r="G4" s="1">
         <v>3600</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2" t="b">
+      <c r="H4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>12566</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D5" s="2" t="s">
+      <c r="E5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F5" s="1">
+      <c r="G5" s="1">
         <v>2500</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2" t="b">
+      <c r="H5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2" t="b">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="331.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" ht="331.2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>12567</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="2" t="s">
+      <c r="E6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F6" s="1">
+      <c r="G6" s="1">
         <v>150</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2" t="b">
+      <c r="H6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2" t="b">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="409.6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" ht="409.6" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>12568</v>
       </c>
-      <c r="B7" s="1" t="s">
-        <v>17</v>
+      <c r="B7" s="2" t="s">
+        <v>76</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F7" s="1">
+      <c r="G7" s="1">
         <v>300</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2" t="b">
+      <c r="H7" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2" t="b">
         <v>0</v>
       </c>
     </row>
@@ -999,7 +1035,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>5</v>
@@ -1010,15 +1046,15 @@
         <v>6</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="262.2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>63</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>64</v>
       </c>
     </row>
   </sheetData>
@@ -1042,74 +1078,74 @@
   <sheetData>
     <row r="1" spans="1:2" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="207.6" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="207" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="69" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B7" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="15" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="105" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -1139,16 +1175,16 @@
   <sheetData>
     <row r="1" spans="1:9" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1158,13 +1194,13 @@
     </row>
     <row r="2" spans="1:9" ht="42" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>29</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>30</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="1"/>
@@ -1175,72 +1211,72 @@
     </row>
     <row r="3" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="303.60000000000002" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="124.2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -1269,16 +1305,16 @@
   <sheetData>
     <row r="1" spans="1:9" ht="31.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="9" t="s">
         <v>24</v>
-      </c>
-      <c r="D1" s="9" t="s">
-        <v>25</v>
       </c>
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
@@ -1288,13 +1324,13 @@
     </row>
     <row r="2" spans="1:9" ht="42" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D2" s="5"/>
       <c r="E2" s="1"/>
@@ -1305,72 +1341,72 @@
     </row>
     <row r="3" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D4" s="12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="303.60000000000002" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B6" s="11"/>
       <c r="C6" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D6" s="14" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="124.2" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="D8" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="D8" s="7" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>